<commit_message>
Update unmet demand parameter
</commit_message>
<xml_diff>
--- a/model/Output Files/Output_10_1.xlsx
+++ b/model/Output Files/Output_10_1.xlsx
@@ -19004,7 +19004,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19160,110 +19160,6 @@
         <v>0</v>
       </c>
       <c r="P3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>Industry</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0</v>
-      </c>
-      <c r="M4" t="n">
-        <v>0</v>
-      </c>
-      <c r="N4" t="n">
-        <v>0</v>
-      </c>
-      <c r="O4" t="n">
-        <v>0</v>
-      </c>
-      <c r="P4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>Solar Farm</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0</v>
-      </c>
-      <c r="M5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N5" t="n">
-        <v>0</v>
-      </c>
-      <c r="O5" t="n">
-        <v>0</v>
-      </c>
-      <c r="P5" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>